<commit_message>
feito ajustes pra rodar no not do pai
</commit_message>
<xml_diff>
--- a/planilha_romaneio.xlsx
+++ b/planilha_romaneio.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -745,6 +745,58 @@
       </c>
       <c r="H10" t="inlineStr"/>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>04/10/2024</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>INFORMAÇÕES FALTANTES</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>DDY4C74</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>ESPIRITO SANTO DO PINHAL</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>04/10/2024</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>INFORMAÇÕES FALTANTES</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>EAR7C31</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>AMPARO</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>